<commit_message>
Add check network file
</commit_message>
<xml_diff>
--- a/printers_v2.xlsx
+++ b/printers_v2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13560" windowHeight="9795" tabRatio="855" firstSheet="3" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13560" windowHeight="9795" tabRatio="855"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="1" r:id="rId1"/>
@@ -7051,7 +7051,7 @@
   </sheetPr>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -9259,7 +9259,7 @@
   </sheetPr>
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" ySplit="12" topLeftCell="G13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
@@ -9672,8 +9672,8 @@
   </sheetPr>
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>